<commit_message>
add view tabel laporan lipa 22
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_22.xlsx
+++ b/hasil/2023_01_lipa_22.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>LAPORAN PENANGANAN BANTUAN PANGGILAN / PEMBERITAHUAN</t>
   </si>
@@ -151,16 +151,16 @@
     <t>W6-A4/127/Hk.05/I/2023</t>
   </si>
   <si>
-    <t>04/01/2023</t>
-  </si>
-  <si>
-    <t>17/01/2023</t>
-  </si>
-  <si>
-    <t>05/01/2023</t>
-  </si>
-  <si>
-    <t>06/01/2023</t>
+    <t>2023-01-04</t>
+  </si>
+  <si>
+    <t>2023-01-17</t>
+  </si>
+  <si>
+    <t>2023-01-05</t>
+  </si>
+  <si>
+    <t>2023-01-06</t>
   </si>
   <si>
     <t>PA CIBINONG</t>
@@ -175,10 +175,10 @@
     <t>W10-A20/70/HK.05/I/2023</t>
   </si>
   <si>
-    <t>09/01/2023</t>
-  </si>
-  <si>
-    <t>13/01/2023</t>
+    <t>2023-01-09</t>
+  </si>
+  <si>
+    <t>2023-01-13</t>
   </si>
   <si>
     <t>Mohammad  Aries Ode, S.H</t>
@@ -196,7 +196,7 @@
     <t>W32-A2/79/HK.05/1/2023</t>
   </si>
   <si>
-    <t>11/01/2023</t>
+    <t>2023-01-11</t>
   </si>
   <si>
     <t>PA PALOPO</t>
@@ -211,7 +211,7 @@
     <t>W20-A10/83/HK.05/I/2023</t>
   </si>
   <si>
-    <t>10/01/2023</t>
+    <t>2023-01-10</t>
   </si>
   <si>
     <t>PA LABUHA</t>
@@ -241,13 +241,16 @@
     <t>W20-A3/118/HK.05/I/2023</t>
   </si>
   <si>
-    <t>10/11/2022</t>
-  </si>
-  <si>
-    <t>12/01/2023</t>
-  </si>
-  <si>
-    <t>19/01/2023</t>
+    <t>2022-11-10</t>
+  </si>
+  <si>
+    <t>2023-01-12</t>
+  </si>
+  <si>
+    <t>2023-01-16</t>
+  </si>
+  <si>
+    <t>2023-01-19</t>
   </si>
   <si>
     <t>Pemberitahuan</t>
@@ -277,13 +280,13 @@
     <t>W10-A20/206/HK.05/I/2023</t>
   </si>
   <si>
-    <t>31/01/2023</t>
-  </si>
-  <si>
-    <t>18/01/2023</t>
-  </si>
-  <si>
-    <t>20/01/2023</t>
+    <t>2023-01-31</t>
+  </si>
+  <si>
+    <t>2023-01-18</t>
+  </si>
+  <si>
+    <t>2023-01-20</t>
   </si>
   <si>
     <t>W29-A3/08/HK.05/I/2023</t>
@@ -301,7 +304,7 @@
     <t>W20-A1/371/Hk.05/I/2023</t>
   </si>
   <si>
-    <t>03/01/2023</t>
+    <t>2023-01-03</t>
   </si>
   <si>
     <t>W29-A3/09/HK.05/I/2023</t>
@@ -310,13 +313,13 @@
     <t>W20-A10/113/HK.05/I/2023</t>
   </si>
   <si>
-    <t>25/01/2023</t>
+    <t>2023-01-25</t>
   </si>
   <si>
     <t>W32-A2/161/HK.05/1/2023</t>
   </si>
   <si>
-    <t>24/01/2023</t>
+    <t>2023-01-24</t>
   </si>
   <si>
     <t>Munira Juniarti, A.Md</t>
@@ -325,7 +328,7 @@
     <t>W.25-A1/0158/HK.05/I/2023</t>
   </si>
   <si>
-    <t>23/01/2023</t>
+    <t>2023-01-23</t>
   </si>
   <si>
     <t>PA PURWOKERTO</t>
@@ -340,7 +343,7 @@
     <t>WII-A22/499/Hk.05/I/2023</t>
   </si>
   <si>
-    <t>28/07/2022</t>
+    <t>2022-07-28</t>
   </si>
   <si>
     <t>PA SOASIO</t>
@@ -364,9 +367,21 @@
     <t>W29-A2/277/HK.05/I/2023</t>
   </si>
   <si>
+    <t>2023-01-26</t>
+  </si>
+  <si>
+    <t>2023-02-07</t>
+  </si>
+  <si>
+    <t>2023-01-27</t>
+  </si>
+  <si>
     <t>W20-A10/162/HK.05/I/2023</t>
   </si>
   <si>
+    <t>2023-01-30</t>
+  </si>
+  <si>
     <t>PA DATARAN HUNIMOA</t>
   </si>
   <si>
@@ -379,13 +394,13 @@
     <t>W24-A5/234/HK.05/I/2023</t>
   </si>
   <si>
-    <t>02/02/2023</t>
+    <t>2023-02-02</t>
   </si>
   <si>
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 02 Agustus 2023</t>
+    <t>Ternate , 11 September 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
@@ -1549,16 +1564,16 @@
         <v>75</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>54</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1566,16 +1581,16 @@
         <v>7</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>64</v>
@@ -1610,13 +1625,13 @@
         <v>65</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>59</v>
@@ -1657,25 +1672,25 @@
         <v>50</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L22" s="12" t="s">
         <v>54</v>
@@ -1692,13 +1707,13 @@
         <v>65</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>45</v>
@@ -1707,22 +1722,22 @@
         <v>64</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L23" s="12" t="s">
         <v>54</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1730,40 +1745,40 @@
         <v>11</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>45</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>54</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1780,31 +1795,31 @@
         <v>67</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>64</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>69</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1821,25 +1836,25 @@
         <v>62</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>45</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>54</v>
@@ -1862,28 +1877,28 @@
         <v>57</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F27" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="H27" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M27" s="12" t="s">
         <v>32</v>
@@ -1894,40 +1909,40 @@
         <v>15</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>52</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>31</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -1935,40 +1950,40 @@
         <v>16</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="J29" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>54</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1976,34 +1991,34 @@
         <v>17</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L30" s="12" t="s">
         <v>31</v>
@@ -2017,37 +2032,37 @@
         <v>18</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M31" s="12" t="s">
         <v>32</v>
@@ -2067,31 +2082,31 @@
         <v>62</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>52</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="L32" s="12" t="s">
         <v>54</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -2099,37 +2114,37 @@
         <v>20</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="12" t="s">
+      <c r="G33" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="I33" s="13" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>32</v>
@@ -2169,7 +2184,7 @@
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="20" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
@@ -2178,7 +2193,7 @@
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
       <c r="J36" s="20" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
@@ -2188,7 +2203,7 @@
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="20" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
@@ -2197,7 +2212,7 @@
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
@@ -2267,7 +2282,7 @@
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
@@ -2276,7 +2291,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
@@ -2286,7 +2301,7 @@
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="20" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
@@ -2295,7 +2310,7 @@
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>

</xml_diff>